<commit_message>
update plot different model_comparison
</commit_message>
<xml_diff>
--- a/result/model_comparison.xlsx
+++ b/result/model_comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiquan/PycharmProjects/antibody project/CoV_Ab_Dataset/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B488A6-FF0A-5346-8F20-1F431CC85DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CB2023-7EC8-1441-AC31-40FC554E083C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14380" xr2:uid="{22B01031-1121-0746-BC5A-A0A49AE0610C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>RBD-HA</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>ROC AUC</t>
+  </si>
+  <si>
+    <t>PR AUC</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9F2D32-7284-7B47-BEA4-8027B340ECEC}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,13 +514,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>0.82224768400000003</v>
+        <v>0.96001636980000005</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -525,10 +528,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>0.85643565649999998</v>
+        <v>0.82224768400000003</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,10 +539,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>0.88415670390000001</v>
+        <v>0.85643565649999998</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,32 +550,32 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>0.87759637830000004</v>
+        <v>0.88415670390000001</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>0.584450423717498</v>
+        <v>0.87759637830000004</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>0.66666668653488104</v>
+        <v>0.93083685640000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,10 +583,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>0.32171583175659102</v>
+        <v>0.62198388576507502</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,10 +594,43 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0.65714287757873502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>0.601307213306427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C13">
-        <v>0.75121468305587702</v>
+      <c r="C15">
+        <v>0.78563416004180897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>0.62366157770156805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>